<commit_message>
work-log updated and did inheritance tasks
</commit_message>
<xml_diff>
--- a/Work-log.xlsx
+++ b/Work-log.xlsx
@@ -120,7 +120,7 @@
     <t>Hankerank tasks on python(strings) and Exceptions</t>
   </si>
   <si>
-    <t>Hankerank tasks on python(sets)</t>
+    <t>Hankerank tasks on python(sets) and Classes</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modified Work-log and added practice files
</commit_message>
<xml_diff>
--- a/Work-log.xlsx
+++ b/Work-log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
   <si>
     <t>CORE TOPIC</t>
   </si>
@@ -120,7 +120,31 @@
     <t>Hankerank tasks on python(strings) and Exceptions</t>
   </si>
   <si>
-    <t>Hankerank tasks on python(sets) and Classes</t>
+    <t>classes inheritances</t>
+  </si>
+  <si>
+    <t>Python/postgresql</t>
+  </si>
+  <si>
+    <t>Hankerank tasks on python(sets)</t>
+  </si>
+  <si>
+    <t>postgresql installation on linux, psycopg2, basic queries,operators,</t>
+  </si>
+  <si>
+    <t>postgresql advanced joins,constraints,</t>
+  </si>
+  <si>
+    <t>off-Sunday</t>
+  </si>
+  <si>
+    <t>*********************</t>
+  </si>
+  <si>
+    <t>practice postgresql with python using an API psycopg2</t>
+  </si>
+  <si>
+    <t>created classes &amp; methods to create table and make CRUD operations on DB(postgresql)</t>
   </si>
 </sst>
 </file>
@@ -536,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -877,7 +901,89 @@
         <v>23</v>
       </c>
       <c r="C30" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="4">
+        <v>43340</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="4">
+        <v>43341</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="4">
+        <v>43342</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="4">
+        <v>43343</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="4">
+        <v>43344</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="4">
+        <v>43345</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="4">
+        <v>43346</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="4">
+        <v>43347</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the work=log and uploaded two file,pip-cmd and pip-doc
</commit_message>
<xml_diff>
--- a/Work-log.xlsx
+++ b/Work-log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="46">
   <si>
     <t>CORE TOPIC</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>created classes &amp; methods to create table and make CRUD operations on DB(postgresql)</t>
+  </si>
+  <si>
+    <t>python/pip</t>
+  </si>
+  <si>
+    <t>pip-intro,installation,requirement files,contraint files,basic commands of pip</t>
+  </si>
+  <si>
+    <t>Created Package and Published the package and then installed it using pip</t>
   </si>
 </sst>
 </file>
@@ -560,17 +569,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
   <cols>
     <col min="1" max="1" width="36.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="110" style="7" customWidth="1"/>
+    <col min="2" max="2" width="31" style="6" customWidth="1"/>
+    <col min="3" max="3" width="119.140625" style="7" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -984,6 +993,28 @@
       </c>
       <c r="C38" s="7" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="4">
+        <v>43348</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="4">
+        <v>43348</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
worklog modified and django cmds file uploaded
</commit_message>
<xml_diff>
--- a/Work-log.xlsx
+++ b/Work-log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
   <si>
     <t>CORE TOPIC</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>installed virtualenv and virtualenvwrapper ,created a virtualenv</t>
+  </si>
+  <si>
+    <t>python-Django</t>
+  </si>
+  <si>
+    <t>installation and basics,,started a polls app project</t>
   </si>
 </sst>
 </file>
@@ -575,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1032,6 +1038,17 @@
       </c>
       <c r="C41" s="7" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="4">
+        <v>43350</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work-log updated and django polls app added
</commit_message>
<xml_diff>
--- a/Work-log.xlsx
+++ b/Work-log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="57">
   <si>
     <t>CORE TOPIC</t>
   </si>
@@ -166,13 +166,34 @@
   </si>
   <si>
     <t>installation and basics,,started a polls app project</t>
+  </si>
+  <si>
+    <t>a polls app project</t>
+  </si>
+  <si>
+    <t>Completed the polls app and created a package of polls app and published,installed it</t>
+  </si>
+  <si>
+    <t>Django polls app project</t>
+  </si>
+  <si>
+    <t>django forms</t>
+  </si>
+  <si>
+    <t>django forms validation</t>
+  </si>
+  <si>
+    <t>LEAVE</t>
+  </si>
+  <si>
+    <t>**********************</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,8 +225,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,8 +277,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5D9F1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD7E4BC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6DDE8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -260,11 +319,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -286,6 +420,27 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:Z48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -947,7 +1102,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:26">
       <c r="A33" s="4">
         <v>43342</v>
       </c>
@@ -958,7 +1113,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:26">
       <c r="A34" s="4">
         <v>43343</v>
       </c>
@@ -969,12 +1124,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:26">
       <c r="A35" s="4">
         <v>43344</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:26">
       <c r="A36" s="4">
         <v>43345</v>
       </c>
@@ -985,7 +1140,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:26">
       <c r="A37" s="4">
         <v>43346</v>
       </c>
@@ -996,7 +1151,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:26">
       <c r="A38" s="4">
         <v>43347</v>
       </c>
@@ -1007,7 +1162,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:26">
       <c r="A39" s="4">
         <v>43348</v>
       </c>
@@ -1018,7 +1173,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:26">
       <c r="A40" s="4">
         <v>43348</v>
       </c>
@@ -1029,7 +1184,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:26">
       <c r="A41" s="4">
         <v>43349</v>
       </c>
@@ -1040,7 +1195,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:26">
       <c r="A42" s="4">
         <v>43350</v>
       </c>
@@ -1050,6 +1205,187 @@
       <c r="C42" s="7" t="s">
         <v>49</v>
       </c>
+    </row>
+    <row r="43" spans="1:26" ht="21.75" thickBot="1">
+      <c r="A43" s="4">
+        <v>43351</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" ht="21.75" thickBot="1">
+      <c r="A44" s="8">
+        <v>43352</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="11"/>
+      <c r="R44" s="11"/>
+      <c r="S44" s="11"/>
+      <c r="T44" s="11"/>
+      <c r="U44" s="11"/>
+      <c r="V44" s="11"/>
+      <c r="W44" s="11"/>
+      <c r="X44" s="11"/>
+      <c r="Y44" s="11"/>
+      <c r="Z44" s="11"/>
+    </row>
+    <row r="45" spans="1:26" ht="21.75" thickBot="1">
+      <c r="A45" s="12">
+        <v>43353</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="11"/>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11"/>
+      <c r="S45" s="11"/>
+      <c r="T45" s="11"/>
+      <c r="U45" s="11"/>
+      <c r="V45" s="11"/>
+      <c r="W45" s="11"/>
+      <c r="X45" s="11"/>
+      <c r="Y45" s="11"/>
+      <c r="Z45" s="11"/>
+    </row>
+    <row r="46" spans="1:26" ht="21.75" thickBot="1">
+      <c r="A46" s="12">
+        <v>43354</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="11"/>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="11"/>
+      <c r="R46" s="11"/>
+      <c r="S46" s="11"/>
+      <c r="T46" s="11"/>
+      <c r="U46" s="11"/>
+      <c r="V46" s="11"/>
+      <c r="W46" s="11"/>
+      <c r="X46" s="11"/>
+      <c r="Y46" s="11"/>
+      <c r="Z46" s="11"/>
+    </row>
+    <row r="47" spans="1:26" ht="21.75" thickBot="1">
+      <c r="A47" s="12">
+        <v>43355</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="11"/>
+      <c r="T47" s="11"/>
+      <c r="U47" s="11"/>
+      <c r="V47" s="11"/>
+      <c r="W47" s="11"/>
+      <c r="X47" s="11"/>
+      <c r="Y47" s="11"/>
+      <c r="Z47" s="11"/>
+    </row>
+    <row r="48" spans="1:26" ht="21.75" thickBot="1">
+      <c r="A48" s="12">
+        <v>43356</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="11"/>
+      <c r="O48" s="11"/>
+      <c r="P48" s="11"/>
+      <c r="Q48" s="11"/>
+      <c r="R48" s="11"/>
+      <c r="S48" s="11"/>
+      <c r="T48" s="11"/>
+      <c r="U48" s="11"/>
+      <c r="V48" s="11"/>
+      <c r="W48" s="11"/>
+      <c r="X48" s="11"/>
+      <c r="Y48" s="11"/>
+      <c r="Z48" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>